<commit_message>
collected more data. New scripts to pulse heating, increase number of sources and time average
</commit_message>
<xml_diff>
--- a/run_log_uniformN.xslx.xlsx
+++ b/run_log_uniformN.xslx.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="191" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="240" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Run Log</t>
   </si>
@@ -32,9 +32,27 @@
     <t>Smooth heating, non Transient, representative of a single convection event in a GCM</t>
   </si>
   <si>
+    <t>narrow heating, non Transient, same total heating</t>
+  </si>
+  <si>
+    <t>Transient heat source</t>
+  </si>
+  <si>
+    <t>Moving Source (around 10ms-1). Keep within grid box</t>
+  </si>
+  <si>
+    <t>2 heat sources alternation on/off</t>
+  </si>
+  <si>
+    <t>2 heat steady sources (sigma 1) vs control</t>
+  </si>
+  <si>
     <t>Sigma (lengthscale)</t>
   </si>
   <si>
+    <t>2x1 vs 5</t>
+  </si>
+  <si>
     <t>no. of modes in heating function</t>
   </si>
   <si>
@@ -63,6 +81,9 @@
   </si>
   <si>
     <t>Total heating conserved</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
   <si>
     <t>converged solution w.r.t. lid height</t>
@@ -80,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -211,10 +233,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -235,7 +257,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -260,178 +282,238 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="C4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="C5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>10000</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>10000</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="5" t="n">
+        <v>10000</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>10000</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>2500</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="n">
+        <v>10000</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>100</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="n">
+        <v>100</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>4</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="G13" s="3" t="n">
-        <v>5</v>
-      </c>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>5</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -444,7 +526,7 @@
     </row>
     <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -455,18 +537,35 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>